<commit_message>
Test engine now directly runs rules from the rule engine. Logic introduced for empty RMRs and for scenarios where multiple elements can pass/fail within the same test.
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/test_generation_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/test_generation_draft.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonz102\Documents\Supriya Work\RCT\rct_test_scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26CD390-ACAA-4CF4-BC03-DFC46298410E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831732D2-C328-497E-BF78-F3229148A5D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="80">
   <si>
     <t>appendix_g_section_id</t>
   </si>
@@ -247,25 +247,9 @@
     <t>key5</t>
   </si>
   <si>
-    <t>id:1,2,3|
-name:Transformer_1,Transformer_2, Transformer_3</t>
-  </si>
-  <si>
     <t>expected_rule_outcome</t>
   </si>
   <si>
-    <t>id:1,2,null|
-name:Transformer_1,Transformer_2,null</t>
-  </si>
-  <si>
-    <t>id:1,2|
-name:Transformer_1,Transformer_2</t>
-  </si>
-  <si>
-    <t>id:1,2|
-name:Transformer_1,Transformer_4</t>
-  </si>
-  <si>
     <t>User RMR transformer name is in the Baseline RMR</t>
   </si>
   <si>
@@ -282,6 +266,21 @@
   </si>
   <si>
     <t>Section</t>
+  </si>
+  <si>
+    <t>name:Transformer_1,Transformer_2, Transformer_3</t>
+  </si>
+  <si>
+    <t>name:Transformer_1,Transformer_2</t>
+  </si>
+  <si>
+    <t>name:Transformer_1,Transformer_4</t>
+  </si>
+  <si>
+    <t>key6</t>
+  </si>
+  <si>
+    <t>key7</t>
   </si>
 </sst>
 </file>
@@ -690,24 +689,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2616CE-C113-4173-BA9E-9D8DBBCAB481}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C8" sqref="C8"/>
+      <pane xSplit="7" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="15" width="55.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="55.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="52.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="53.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="47.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="51.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="47" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>49</v>
       </c>
@@ -723,61 +731,63 @@
       <c r="E1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="8" t="str">
-        <f>"rule-"&amp;F2&amp;"-"&amp;F3&amp;F4</f>
+      <c r="F1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="8" t="str">
+        <f>"rule-"&amp;H2&amp;"-"&amp;H3&amp;H4</f>
         <v>rule-15-1a</v>
       </c>
-      <c r="G1" s="8" t="str">
-        <f t="shared" ref="G1:K1" si="0">"rule-"&amp;G2&amp;"-"&amp;G3&amp;G4</f>
+      <c r="I1" s="8" t="str">
+        <f t="shared" ref="I1:M1" si="0">"rule-"&amp;I2&amp;"-"&amp;I3&amp;I4</f>
         <v>rule-15-1b</v>
       </c>
-      <c r="H1" s="8" t="str">
+      <c r="J1" s="8" t="str">
         <f t="shared" si="0"/>
         <v>rule-15-1c</v>
       </c>
-      <c r="I1" s="8" t="str">
+      <c r="K1" s="8" t="str">
         <f t="shared" si="0"/>
         <v>rule-15-2a</v>
       </c>
-      <c r="J1" s="8" t="str">
+      <c r="L1" s="8" t="str">
         <f t="shared" si="0"/>
         <v>rule-15-2b</v>
       </c>
-      <c r="K1" s="8" t="str">
+      <c r="M1" s="8" t="str">
         <f t="shared" si="0"/>
         <v>rule-15-2c</v>
       </c>
-      <c r="L1" s="8" t="str">
-        <f t="shared" ref="L1:M1" si="1">"rule-"&amp;L2&amp;"-"&amp;L3&amp;L4</f>
+      <c r="N1" s="8" t="str">
+        <f t="shared" ref="N1:O1" si="1">"rule-"&amp;N2&amp;"-"&amp;N3&amp;N4</f>
         <v>rule-15-3a</v>
       </c>
-      <c r="M1" s="8" t="str">
+      <c r="O1" s="8" t="str">
         <f t="shared" si="1"/>
         <v>rule-15-3b</v>
       </c>
-      <c r="N1" s="8" t="str">
-        <f t="shared" ref="N1:O1" si="2">"rule-"&amp;N2&amp;"-"&amp;N3&amp;N4</f>
+      <c r="P1" s="8" t="str">
+        <f t="shared" ref="P1:Q1" si="2">"rule-"&amp;P2&amp;"-"&amp;P3&amp;P4</f>
         <v>rule-15-4a</v>
       </c>
-      <c r="O1" s="8" t="str">
+      <c r="Q1" s="8" t="str">
         <f t="shared" si="2"/>
         <v>rule-15-4b</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="4">
-        <v>15</v>
-      </c>
-      <c r="G2" s="4">
-        <v>15</v>
-      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="4">
         <v>15</v>
       </c>
@@ -802,8 +812,14 @@
       <c r="O2" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>47</v>
       </c>
@@ -811,38 +827,40 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="4">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1</v>
-      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="4">
         <v>1</v>
       </c>
       <c r="I3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" s="4">
         <v>2</v>
       </c>
       <c r="L3" s="4">
+        <v>2</v>
+      </c>
+      <c r="M3" s="4">
+        <v>2</v>
+      </c>
+      <c r="N3" s="4">
         <v>3</v>
       </c>
-      <c r="M3" s="4">
+      <c r="O3" s="4">
         <v>3</v>
       </c>
-      <c r="N3" s="4">
+      <c r="P3" s="4">
         <v>4</v>
       </c>
-      <c r="O3" s="4">
+      <c r="Q3" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>55</v>
       </c>
@@ -850,29 +868,25 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>8</v>
@@ -880,8 +894,14 @@
       <c r="O4" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="P4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>52</v>
       </c>
@@ -889,58 +909,64 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="N5" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="P5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>65</v>
       </c>
@@ -951,41 +977,43 @@
         <v>57</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="I8" s="9" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>65</v>
       </c>
@@ -996,26 +1024,28 @@
         <v>57</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="K9" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="I9" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="L9" s="9" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>65</v>
       </c>
@@ -1026,56 +1056,54 @@
         <v>57</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="9" t="s">
+      <c r="I10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="O10" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="K11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>20</v>
@@ -1086,108 +1114,142 @@
       <c r="O11" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:O11" xr:uid="{AF93CD98-D7BE-4C5E-872E-43CDD83EAE71}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H11:Q11" xr:uid="{AF93CD98-D7BE-4C5E-872E-43CDD83EAE71}">
       <formula1>TEST_OUTCOME_TYPES</formula1>
     </dataValidation>
   </dataValidations>
@@ -1433,7 +1495,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>